<commit_message>
ontoclean for trans + update on scal
</commit_message>
<xml_diff>
--- a/ontologies/scal_punned.xlsx
+++ b/ontologies/scal_punned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gruber04\git_repos\PhD\phd_semantic_init\ontologies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26BE643-8228-41B1-8788-5CDE5266B0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B77CB1C-A665-4D11-8065-F7B6691E5631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33735" yWindow="-1785" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37620" yWindow="-585" windowWidth="19305" windowHeight="15270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="preamble" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="75">
   <si>
     <t>a</t>
   </si>
@@ -101,9 +101,6 @@
   </si>
   <si>
     <t>~U</t>
-  </si>
-  <si>
-    <t>-U</t>
   </si>
   <si>
     <t>Assumed external meta properties</t>
@@ -586,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E1118D-B656-475B-8493-F4267084EC82}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -600,262 +597,262 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
         <v>64</v>
-      </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
         <v>34</v>
       </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
         <v>40</v>
       </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
         <v>42</v>
       </c>
-      <c r="C8" t="s">
-        <v>43</v>
-      </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
         <v>44</v>
       </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
         <v>46</v>
       </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" t="s">
-        <v>49</v>
-      </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
         <v>52</v>
       </c>
-      <c r="C13" t="s">
-        <v>53</v>
-      </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
         <v>54</v>
       </c>
-      <c r="C15" t="s">
-        <v>55</v>
-      </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
       </c>
       <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s">
         <v>56</v>
-      </c>
-      <c r="D17" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
         <v>59</v>
       </c>
-      <c r="C19" t="s">
-        <v>60</v>
-      </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -871,15 +868,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" customWidth="1"/>
     <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -888,22 +886,22 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
         <v>70</v>
       </c>
-      <c r="C1" t="s">
-        <v>71</v>
-      </c>
       <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
         <v>66</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>68</v>
-      </c>
-      <c r="G1" t="s">
-        <v>69</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
@@ -923,13 +921,13 @@
         <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -949,7 +947,7 @@
         <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -969,7 +967,7 @@
         <v>17</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -989,7 +987,7 @@
         <v>17</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1009,7 +1007,7 @@
         <v>17</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1029,7 +1027,7 @@
         <v>17</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1049,7 +1047,7 @@
         <v>17</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1072,7 +1070,7 @@
         <v>21</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1080,7 +1078,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>16</v>
@@ -1095,7 +1093,7 @@
         <v>17</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1103,7 +1101,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>16</v>
@@ -1112,13 +1110,13 @@
         <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1126,7 +1124,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>16</v>
@@ -1141,7 +1139,7 @@
         <v>21</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1164,7 +1162,7 @@
         <v>21</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1178,13 +1176,13 @@
         <v>20</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1207,7 +1205,7 @@
         <v>17</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1230,7 +1228,7 @@
         <v>17</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>